<commit_message>
Actualizacion Test_AWS - Test 2
</commit_message>
<xml_diff>
--- a/Test_AWS/NUEVO_COMBI.xlsx
+++ b/Test_AWS/NUEVO_COMBI.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -393,10 +393,10 @@
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">

</xml_diff>